<commit_message>
complete update to visualisation
</commit_message>
<xml_diff>
--- a/11-Parameters/HorizRight-BeamLine-Gauss-Solenoid.xlsx
+++ b/11-Parameters/HorizRight-BeamLine-Gauss-Solenoid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942E0D99-3E85-D144-900D-C71A7C5218DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C71A33-9B79-084D-B36B-584F0D521CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="640" windowWidth="18500" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8680" yWindow="1060" windowWidth="18500" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LhARABeamLine-Params-LsrDrvn" sheetId="1" r:id="rId1"/>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>